<commit_message>
readme update and forward test image
</commit_message>
<xml_diff>
--- a/ManualFiles/Forward_Test_Results.xlsx
+++ b/ManualFiles/Forward_Test_Results.xlsx
@@ -57,7 +57,7 @@
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -107,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -116,26 +116,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -231,6 +211,19 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -244,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -254,68 +247,74 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -473,16 +472,16 @@
                   <c:v>1.0106982294917519</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0146679718674565</c:v>
+                  <c:v>1.0106982294917519</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0173144667845928</c:v>
+                  <c:v>1.0133343703784949</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0162603451216639</c:v>
+                  <c:v>1.0133343703784949</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0162603451216639</c:v>
+                  <c:v>1.0187686816529296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -584,22 +583,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.002960520642058</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0077148688212978</c:v>
+                  <c:v>1.0106982294917519</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0077148688212978</c:v>
+                  <c:v>1.0146679718674565</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0103432283952674</c:v>
+                  <c:v>1.0146679718674565</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0103432283952674</c:v>
+                  <c:v>1.0136165924516045</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0103432283952674</c:v>
+                  <c:v>1.0136165924516045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -734,11 +733,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116753920"/>
-        <c:axId val="116755456"/>
+        <c:axId val="106494592"/>
+        <c:axId val="106377600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116753920"/>
+        <c:axId val="106494592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +747,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116755456"/>
+        <c:crossAx val="106377600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -756,7 +755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116755456"/>
+        <c:axId val="106377600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,7 +784,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116753920"/>
+        <c:crossAx val="106494592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -823,16 +822,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600073</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:colOff>1237867</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1141,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L31"/>
+  <dimension ref="B2:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,700 +1164,301 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:12" s="8" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+    <row r="3" spans="2:12" s="5" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="13">
+      <c r="B4" s="10">
         <v>44484</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16">
-        <v>1</v>
-      </c>
-      <c r="K4" s="16">
-        <v>1</v>
-      </c>
-      <c r="L4" s="17">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13">
+        <v>1</v>
+      </c>
+      <c r="K4" s="13">
+        <v>1</v>
+      </c>
+      <c r="L4" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="18">
+      <c r="B5" s="15">
         <v>44487</v>
       </c>
-      <c r="C5" s="19">
-        <v>1</v>
-      </c>
-      <c r="D5" s="19">
-        <v>0</v>
-      </c>
-      <c r="E5" s="20">
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17">
         <v>447.19000244140602</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="18">
         <v>2.96052064205798E-3</v>
       </c>
-      <c r="G5" s="19">
-        <v>1</v>
-      </c>
-      <c r="H5" s="21">
+      <c r="G5" s="16">
+        <v>1</v>
+      </c>
+      <c r="H5" s="18">
         <f>C5*F5</f>
         <v>2.96052064205798E-3</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="18">
         <f>D5*F5</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="22">
+        <v>2.96052064205798E-3</v>
+      </c>
+      <c r="J5" s="19">
         <f t="shared" ref="J5:K9" si="0">J4*(1+H5)</f>
         <v>1.002960520642058</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L5" s="23">
-        <f>L4*(1+F5)</f>
+        <v>1.002960520642058</v>
+      </c>
+      <c r="L5" s="20">
+        <f t="shared" ref="L5:L10" si="1">L4*(1+F5)</f>
         <v>1.002960520642058</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="13">
+      <c r="B6" s="10">
         <v>44488</v>
       </c>
-      <c r="C6" s="14">
-        <v>1</v>
-      </c>
-      <c r="D6" s="14">
-        <v>1</v>
-      </c>
-      <c r="E6" s="24">
+      <c r="C6" s="11">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1</v>
+      </c>
+      <c r="E6" s="21">
         <v>450.64001464843699</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <v>7.7148688212977899E-3</v>
       </c>
-      <c r="G6" s="14">
-        <v>1</v>
-      </c>
-      <c r="H6" s="25">
-        <f t="shared" ref="H6:H9" si="1">C6*F6</f>
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+      <c r="H6" s="22">
+        <f t="shared" ref="H6:H9" si="2">C6*F6</f>
         <v>7.7148688212977899E-3</v>
       </c>
-      <c r="I6" s="25">
-        <f t="shared" ref="I6:I9" si="2">D6*F6</f>
+      <c r="I6" s="22">
+        <f t="shared" ref="I6:I9" si="3">D6*F6</f>
         <v>7.7148688212977899E-3</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="13">
         <f t="shared" si="0"/>
         <v>1.0106982294917519</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="13">
         <f t="shared" si="0"/>
-        <v>1.0077148688212978</v>
-      </c>
-      <c r="L6" s="17">
-        <f>L5*(1+F6)</f>
+        <v>1.0106982294917519</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" si="1"/>
         <v>1.0106982294917519</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="18">
+      <c r="B7" s="15">
         <v>44489</v>
       </c>
-      <c r="C7" s="19">
-        <v>1</v>
-      </c>
-      <c r="D7" s="19">
+      <c r="C7" s="16">
         <v>0</v>
       </c>
-      <c r="E7" s="20">
+      <c r="D7" s="16">
+        <v>1</v>
+      </c>
+      <c r="E7" s="17">
         <v>452.41000366210898</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="18">
         <v>3.9277226969129898E-3</v>
       </c>
-      <c r="G7" s="19">
-        <v>1</v>
-      </c>
-      <c r="H7" s="21">
-        <f t="shared" si="1"/>
-        <v>3.9277226969129898E-3</v>
-      </c>
-      <c r="I7" s="21">
+      <c r="G7" s="16">
+        <v>1</v>
+      </c>
+      <c r="H7" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J7" s="22">
+      <c r="I7" s="18">
+        <f t="shared" si="3"/>
+        <v>3.9277226969129898E-3</v>
+      </c>
+      <c r="J7" s="19">
+        <f t="shared" si="0"/>
+        <v>1.0106982294917519</v>
+      </c>
+      <c r="K7" s="19">
         <f t="shared" si="0"/>
         <v>1.0146679718674565</v>
       </c>
-      <c r="K7" s="22">
-        <f t="shared" si="0"/>
-        <v>1.0077148688212978</v>
-      </c>
-      <c r="L7" s="23">
-        <f>L6*(1+F7)</f>
+      <c r="L7" s="20">
+        <f t="shared" si="1"/>
         <v>1.0146679718674565</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="13">
+      <c r="B8" s="10">
         <v>44490</v>
       </c>
-      <c r="C8" s="14">
-        <v>1</v>
-      </c>
-      <c r="D8" s="14">
-        <v>1</v>
-      </c>
-      <c r="E8" s="24">
+      <c r="C8" s="11">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="21">
         <v>453.58999633789</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>2.6082373648450498E-3</v>
       </c>
-      <c r="G8" s="14">
-        <v>1</v>
-      </c>
-      <c r="H8" s="25">
-        <f t="shared" si="1"/>
-        <v>2.6082373648450498E-3</v>
-      </c>
-      <c r="I8" s="25">
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="22">
         <f t="shared" si="2"/>
         <v>2.6082373648450498E-3</v>
       </c>
-      <c r="J8" s="16">
+      <c r="I8" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
         <f t="shared" si="0"/>
-        <v>1.0173144667845928</v>
-      </c>
-      <c r="K8" s="16">
+        <v>1.0133343703784949</v>
+      </c>
+      <c r="K8" s="13">
         <f t="shared" si="0"/>
-        <v>1.0103432283952674</v>
-      </c>
-      <c r="L8" s="17">
-        <f>L7*(1+F8)</f>
+        <v>1.0146679718674565</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="1"/>
         <v>1.0173144667845928</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="18">
+      <c r="B9" s="15">
         <v>44491</v>
       </c>
-      <c r="C9" s="19">
-        <v>1</v>
-      </c>
-      <c r="D9" s="19">
+      <c r="C9" s="16">
         <v>0</v>
       </c>
-      <c r="E9" s="20">
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="17">
         <v>453.11999511718699</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="18">
         <v>-1.0361807458226699E-3</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="16">
         <v>0</v>
       </c>
-      <c r="H9" s="21">
-        <f t="shared" si="1"/>
-        <v>-1.0361807458226699E-3</v>
-      </c>
-      <c r="I9" s="21">
+      <c r="H9" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J9" s="22">
+      <c r="I9" s="18">
+        <f t="shared" si="3"/>
+        <v>-1.0361807458226699E-3</v>
+      </c>
+      <c r="J9" s="19">
         <f t="shared" si="0"/>
+        <v>1.0133343703784949</v>
+      </c>
+      <c r="K9" s="19">
+        <f t="shared" si="0"/>
+        <v>1.0136165924516045</v>
+      </c>
+      <c r="L9" s="20">
+        <f t="shared" si="1"/>
         <v>1.0162603451216639</v>
       </c>
-      <c r="K9" s="22">
-        <f t="shared" si="0"/>
-        <v>1.0103432283952674</v>
-      </c>
-      <c r="L9" s="23">
-        <f>L8*(1+F9)</f>
-        <v>1.0162603451216639</v>
-      </c>
     </row>
-    <row r="10" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="13">
+    <row r="10" spans="2:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="23">
         <v>44494</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="24">
+        <v>1</v>
+      </c>
+      <c r="D10" s="24">
         <v>0</v>
       </c>
-      <c r="D10" s="14">
+      <c r="E10" s="25">
+        <v>455.54998779296801</v>
+      </c>
+      <c r="F10" s="26">
+        <v>5.36280169042813E-3</v>
+      </c>
+      <c r="G10" s="24">
+        <v>1</v>
+      </c>
+      <c r="H10" s="26">
+        <f t="shared" ref="H10" si="4">C10*F10</f>
+        <v>5.36280169042813E-3</v>
+      </c>
+      <c r="I10" s="26">
+        <f t="shared" ref="I10" si="5">D10*F10</f>
         <v>0</v>
       </c>
-      <c r="E10" s="24">
-        <v>455.54998779296801</v>
-      </c>
-      <c r="F10" s="25">
-        <v>5.36280169042813E-3</v>
-      </c>
-      <c r="G10" s="14">
-        <v>1</v>
-      </c>
-      <c r="H10" s="25">
-        <f t="shared" ref="H10" si="3">C10*F10</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="25">
-        <f t="shared" ref="I10" si="4">D10*F10</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="16">
-        <f t="shared" ref="J10" si="5">J9*(1+H10)</f>
-        <v>1.0162603451216639</v>
-      </c>
-      <c r="K10" s="16">
-        <f t="shared" ref="K10" si="6">K9*(1+I10)</f>
-        <v>1.0103432283952674</v>
-      </c>
-      <c r="L10" s="17">
-        <f>L9*(1+F10)</f>
+      <c r="J10" s="27">
+        <f t="shared" ref="J10" si="6">J9*(1+H10)</f>
+        <v>1.0187686816529296</v>
+      </c>
+      <c r="K10" s="27">
+        <f t="shared" ref="K10" si="7">K9*(1+I10)</f>
+        <v>1.0136165924516045</v>
+      </c>
+      <c r="L10" s="28">
+        <f t="shared" si="1"/>
         <v>1.0217103478183973</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="18">
-        <v>44495</v>
-      </c>
-      <c r="C11" s="19">
-        <v>1</v>
-      </c>
-      <c r="D11" s="19">
-        <v>1</v>
-      </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="28"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="18">
-        <v>44496</v>
-      </c>
-      <c r="C12" s="19">
-        <v>1</v>
-      </c>
-      <c r="D12" s="19">
-        <v>0</v>
-      </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="28"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="18">
-        <v>44497</v>
-      </c>
-      <c r="C13" s="19">
-        <v>1</v>
-      </c>
-      <c r="D13" s="19">
-        <v>1</v>
-      </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="28"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="18">
-        <v>44498</v>
-      </c>
-      <c r="C14" s="19">
-        <v>1</v>
-      </c>
-      <c r="D14" s="19">
-        <v>1</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="28"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="18">
-        <v>44501</v>
-      </c>
-      <c r="C15" s="19">
-        <v>0</v>
-      </c>
-      <c r="D15" s="19">
-        <v>1</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="28"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="18">
-        <v>44502</v>
-      </c>
-      <c r="C16" s="19">
-        <v>1</v>
-      </c>
-      <c r="D16" s="19">
-        <v>0</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="28"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="18">
-        <v>44503</v>
-      </c>
-      <c r="C17" s="19">
-        <v>0</v>
-      </c>
-      <c r="D17" s="19">
-        <v>0</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="28"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="18">
-        <v>44504</v>
-      </c>
-      <c r="C18" s="19">
-        <v>0</v>
-      </c>
-      <c r="D18" s="19">
-        <v>1</v>
-      </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="28"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="18">
-        <v>44505</v>
-      </c>
-      <c r="C19" s="19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="28"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="18">
-        <v>44508</v>
-      </c>
-      <c r="C20" s="19">
-        <v>1</v>
-      </c>
-      <c r="D20" s="19">
-        <v>1</v>
-      </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="28"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="18">
-        <v>44509</v>
-      </c>
-      <c r="C21" s="19">
-        <v>0</v>
-      </c>
-      <c r="D21" s="19">
-        <v>0</v>
-      </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="28"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="18">
-        <v>44510</v>
-      </c>
-      <c r="C22" s="19">
-        <v>1</v>
-      </c>
-      <c r="D22" s="19">
-        <v>1</v>
-      </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="28"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="18">
-        <v>44511</v>
-      </c>
-      <c r="C23" s="19">
-        <v>1</v>
-      </c>
-      <c r="D23" s="19">
-        <v>1</v>
-      </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="28"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="18">
-        <v>44512</v>
-      </c>
-      <c r="C24" s="19">
-        <v>0</v>
-      </c>
-      <c r="D24" s="19">
-        <v>0</v>
-      </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="28"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="18">
-        <v>44515</v>
-      </c>
-      <c r="C25" s="19">
-        <v>0</v>
-      </c>
-      <c r="D25" s="19">
-        <v>0</v>
-      </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="28"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="18">
-        <v>44516</v>
-      </c>
-      <c r="C26" s="19">
-        <v>0</v>
-      </c>
-      <c r="D26" s="19">
-        <v>1</v>
-      </c>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="28"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="18">
-        <v>44517</v>
-      </c>
-      <c r="C27" s="19">
-        <v>0</v>
-      </c>
-      <c r="D27" s="19">
-        <v>0</v>
-      </c>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="28"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="18">
-        <v>44518</v>
-      </c>
-      <c r="C28" s="19">
-        <v>1</v>
-      </c>
-      <c r="D28" s="19">
-        <v>0</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="28"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="18">
-        <v>44519</v>
-      </c>
-      <c r="C29" s="19">
-        <v>1</v>
-      </c>
-      <c r="D29" s="19">
-        <v>1</v>
-      </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="28"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="18">
-        <v>44522</v>
-      </c>
-      <c r="C30" s="19">
-        <v>1</v>
-      </c>
-      <c r="D30" s="19">
-        <v>1</v>
-      </c>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="28"/>
-    </row>
-    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="29">
-        <v>44523</v>
-      </c>
-      <c r="C31" s="30">
-        <v>1</v>
-      </c>
-      <c r="D31" s="30">
-        <v>1</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>